<commit_message>
changes before i start looping
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1151,7 +1151,7 @@
         <v>24.65</v>
       </c>
       <c r="G2" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-15119</v>
       </c>
       <c r="H2" t="n">
         <v>255256</v>
@@ -1183,7 +1183,7 @@
         <v>24.66</v>
       </c>
       <c r="G3" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-15279</v>
       </c>
       <c r="H3" t="n">
         <v>256218</v>
@@ -1215,7 +1215,7 @@
         <v>24.79</v>
       </c>
       <c r="G4" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-15439</v>
       </c>
       <c r="H4" t="n">
         <v>257180</v>
@@ -1247,7 +1247,7 @@
         <v>24.91</v>
       </c>
       <c r="G5" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-15599</v>
       </c>
       <c r="H5" t="n">
         <v>258142</v>
@@ -1279,7 +1279,7 @@
         <v>24.69</v>
       </c>
       <c r="G6" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-15086.6666666667</v>
       </c>
       <c r="H6" t="n">
         <v>259164</v>
@@ -1311,7 +1311,7 @@
         <v>24.5</v>
       </c>
       <c r="G7" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-14574.3333333333</v>
       </c>
       <c r="H7" t="n">
         <v>260186</v>
@@ -1343,7 +1343,7 @@
         <v>24.4</v>
       </c>
       <c r="G8" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-14062</v>
       </c>
       <c r="H8" t="n">
         <v>261208</v>
@@ -1375,7 +1375,7 @@
         <v>24.46</v>
       </c>
       <c r="G9" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-14367.6666666667</v>
       </c>
       <c r="H9" t="n">
         <v>261965.333333333</v>
@@ -1407,7 +1407,7 @@
         <v>24.88</v>
       </c>
       <c r="G10" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-14673.3333333333</v>
       </c>
       <c r="H10" t="n">
         <v>262722.666666667</v>
@@ -1439,7 +1439,7 @@
         <v>24.94</v>
       </c>
       <c r="G11" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-14979</v>
       </c>
       <c r="H11" t="n">
         <v>263480</v>
@@ -1471,7 +1471,7 @@
         <v>25.08</v>
       </c>
       <c r="G12" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-13921</v>
       </c>
       <c r="H12" t="n">
         <v>264460</v>
@@ -1503,7 +1503,7 @@
         <v>25.06</v>
       </c>
       <c r="G13" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-12863</v>
       </c>
       <c r="H13" t="n">
         <v>265440</v>
@@ -1535,7 +1535,7 @@
         <v>25.12</v>
       </c>
       <c r="G14" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-11805</v>
       </c>
       <c r="H14" t="n">
         <v>266420</v>
@@ -1567,7 +1567,7 @@
         <v>25.14</v>
       </c>
       <c r="G15" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-11275.3333333333</v>
       </c>
       <c r="H15" t="n">
         <v>267785</v>
@@ -1599,7 +1599,7 @@
         <v>25.19</v>
       </c>
       <c r="G16" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-10745.6666666667</v>
       </c>
       <c r="H16" t="n">
         <v>269150</v>
@@ -1631,7 +1631,7 @@
         <v>25.2</v>
       </c>
       <c r="G17" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-10216</v>
       </c>
       <c r="H17" t="n">
         <v>270515</v>
@@ -1663,7 +1663,7 @@
         <v>24.99</v>
       </c>
       <c r="G18" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-9993.66666666667</v>
       </c>
       <c r="H18" t="n">
         <v>271442.333333333</v>
@@ -1695,7 +1695,7 @@
         <v>24.97</v>
       </c>
       <c r="G19" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-9771.33333333333</v>
       </c>
       <c r="H19" t="n">
         <v>272369.666666667</v>
@@ -1727,7 +1727,7 @@
         <v>24.79</v>
       </c>
       <c r="G20" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-9549</v>
       </c>
       <c r="H20" t="n">
         <v>273297</v>
@@ -1759,7 +1759,7 @@
         <v>24.93</v>
       </c>
       <c r="G21" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-11269</v>
       </c>
       <c r="H21" t="n">
         <v>274205</v>
@@ -1791,7 +1791,7 @@
         <v>25.47</v>
       </c>
       <c r="G22" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-12989</v>
       </c>
       <c r="H22" t="n">
         <v>275113</v>
@@ -1823,7 +1823,7 @@
         <v>25.41</v>
       </c>
       <c r="G23" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-14709</v>
       </c>
       <c r="H23" t="n">
         <v>276021</v>
@@ -1855,7 +1855,7 @@
         <v>25.47</v>
       </c>
       <c r="G24" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-16245.6666666667</v>
       </c>
       <c r="H24" t="n">
         <v>276119.333333333</v>
@@ -1887,7 +1887,7 @@
         <v>25.49</v>
       </c>
       <c r="G25" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-17782.3333333333</v>
       </c>
       <c r="H25" t="n">
         <v>276217.666666667</v>
@@ -1919,7 +1919,7 @@
         <v>25.65</v>
       </c>
       <c r="G26" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-19319</v>
       </c>
       <c r="H26" t="n">
         <v>276316</v>
@@ -1951,7 +1951,7 @@
         <v>25.63</v>
       </c>
       <c r="G27" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-18430.6666666667</v>
       </c>
       <c r="H27" t="n">
         <v>277061</v>
@@ -1983,7 +1983,7 @@
         <v>25.66</v>
       </c>
       <c r="G28" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-17542.3333333333</v>
       </c>
       <c r="H28" t="n">
         <v>277806</v>
@@ -2015,7 +2015,7 @@
         <v>25.83</v>
       </c>
       <c r="G29" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-16654</v>
       </c>
       <c r="H29" t="n">
         <v>278551</v>
@@ -2047,7 +2047,7 @@
         <v>25.69</v>
       </c>
       <c r="G30" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-16330.3333333333</v>
       </c>
       <c r="H30" t="n">
         <v>279831.333333333</v>
@@ -2079,13 +2079,13 @@
         <v>25.73</v>
       </c>
       <c r="G31" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-16006.6666666667</v>
       </c>
       <c r="H31" t="n">
         <v>281111.666666667</v>
       </c>
       <c r="I31" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-2693.66666666667</v>
       </c>
       <c r="J31" t="n">
         <v>0.7464</v>
@@ -2111,13 +2111,13 @@
         <v>25.7</v>
       </c>
       <c r="G32" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-15683</v>
       </c>
       <c r="H32" t="n">
         <v>282392</v>
       </c>
       <c r="I32" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-8534</v>
       </c>
       <c r="J32" t="n">
         <v>0.5019</v>
@@ -2143,13 +2143,13 @@
         <v>25.73</v>
       </c>
       <c r="G33" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-16426.3333333333</v>
       </c>
       <c r="H33" t="n">
         <v>283201.333333333</v>
       </c>
       <c r="I33" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-7678</v>
       </c>
       <c r="J33" t="n">
         <v>0.5026</v>
@@ -2175,13 +2175,13 @@
         <v>26.14</v>
       </c>
       <c r="G34" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-17169.6666666667</v>
       </c>
       <c r="H34" t="n">
         <v>284010.666666667</v>
       </c>
       <c r="I34" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-6822</v>
       </c>
       <c r="J34" t="n">
         <v>0.5002</v>
@@ -2207,13 +2207,13 @@
         <v>26.21</v>
       </c>
       <c r="G35" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-17913</v>
       </c>
       <c r="H35" t="n">
         <v>284820</v>
       </c>
       <c r="I35" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-5966</v>
       </c>
       <c r="J35" t="n">
         <v>0.4991</v>
@@ -2239,13 +2239,13 @@
         <v>26.29</v>
       </c>
       <c r="G36" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-18156</v>
       </c>
       <c r="H36" t="n">
         <v>284978.666666667</v>
       </c>
       <c r="I36" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-5494.33333333333</v>
       </c>
       <c r="J36" t="n">
         <v>0.4967</v>
@@ -2271,13 +2271,13 @@
         <v>26.26</v>
       </c>
       <c r="G37" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-18399</v>
       </c>
       <c r="H37" t="n">
         <v>285137.333333333</v>
       </c>
       <c r="I37" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-5022.66666666667</v>
       </c>
       <c r="J37" t="n">
         <v>0.5242</v>
@@ -2303,13 +2303,13 @@
         <v>26.41</v>
       </c>
       <c r="G38" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-18642</v>
       </c>
       <c r="H38" t="n">
         <v>285296</v>
       </c>
       <c r="I38" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-4551</v>
       </c>
       <c r="J38" t="n">
         <v>0.5153</v>
@@ -2335,13 +2335,13 @@
         <v>26.45</v>
       </c>
       <c r="G39" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-18363.6666666667</v>
       </c>
       <c r="H39" t="n">
         <v>285784</v>
       </c>
       <c r="I39" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-1143.66666666667</v>
       </c>
       <c r="J39" t="n">
         <v>0.4991</v>
@@ -2367,7 +2367,7 @@
         <v>26.52</v>
       </c>
       <c r="G40" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-18085.3333333333</v>
       </c>
       <c r="H40" t="n">
         <v>286272</v>
@@ -2399,7 +2399,7 @@
         <v>26.55</v>
       </c>
       <c r="G41" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-17807</v>
       </c>
       <c r="H41" t="n">
         <v>286760</v>
@@ -2431,7 +2431,7 @@
         <v>26.22</v>
       </c>
       <c r="G42" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-17341.6666666667</v>
       </c>
       <c r="H42" t="n">
         <v>287517.666666667</v>
@@ -2463,7 +2463,7 @@
         <v>26.14</v>
       </c>
       <c r="G43" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-16876.3333333333</v>
       </c>
       <c r="H43" t="n">
         <v>288275.333333333</v>
@@ -2495,7 +2495,7 @@
         <v>26.08</v>
       </c>
       <c r="G44" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-16411</v>
       </c>
       <c r="H44" t="n">
         <v>289033</v>
@@ -2527,7 +2527,7 @@
         <v>26.13</v>
       </c>
       <c r="G45" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-14171.6666666667</v>
       </c>
       <c r="H45" t="n">
         <v>290215</v>
@@ -2559,7 +2559,7 @@
         <v>26.53</v>
       </c>
       <c r="G46" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-11932.3333333333</v>
       </c>
       <c r="H46" t="n">
         <v>291397</v>
@@ -2591,13 +2591,13 @@
         <v>26.59</v>
       </c>
       <c r="G47" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-9693</v>
       </c>
       <c r="H47" t="n">
         <v>292579</v>
       </c>
       <c r="I47" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-3057</v>
       </c>
       <c r="J47" t="n">
         <v>0.4883</v>
@@ -2623,7 +2623,7 @@
         <v>26.65</v>
       </c>
       <c r="G48" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-10654</v>
       </c>
       <c r="H48" t="n">
         <v>294041.666666667</v>
@@ -2655,7 +2655,7 @@
         <v>26.62</v>
       </c>
       <c r="G49" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-11615</v>
       </c>
       <c r="H49" t="n">
         <v>295504.333333333</v>
@@ -2687,7 +2687,7 @@
         <v>26.68</v>
       </c>
       <c r="G50" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-12576</v>
       </c>
       <c r="H50" t="n">
         <v>296967</v>
@@ -2719,7 +2719,7 @@
         <v>26.77</v>
       </c>
       <c r="G51" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-13370</v>
       </c>
       <c r="H51" t="n">
         <v>298332</v>
@@ -2751,7 +2751,7 @@
         <v>26.82</v>
       </c>
       <c r="G52" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-14164</v>
       </c>
       <c r="H52" t="n">
         <v>299697</v>
@@ -2783,7 +2783,7 @@
         <v>26.77</v>
       </c>
       <c r="G53" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-14958</v>
       </c>
       <c r="H53" t="n">
         <v>301062</v>
@@ -2815,7 +2815,7 @@
         <v>26.57</v>
       </c>
       <c r="G54" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-15581.3333333333</v>
       </c>
       <c r="H54" t="n">
         <v>301888.333333333</v>
@@ -2847,7 +2847,7 @@
         <v>26.56</v>
       </c>
       <c r="G55" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-16204.6666666667</v>
       </c>
       <c r="H55" t="n">
         <v>302714.666666667</v>
@@ -2879,7 +2879,7 @@
         <v>26.49</v>
       </c>
       <c r="G56" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-16828</v>
       </c>
       <c r="H56" t="n">
         <v>303541</v>
@@ -2911,7 +2911,7 @@
         <v>26.66</v>
       </c>
       <c r="G57" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-16431</v>
       </c>
       <c r="H57" t="n">
         <v>304888.333333333</v>
@@ -2943,7 +2943,7 @@
         <v>27.05</v>
       </c>
       <c r="G58" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-16034</v>
       </c>
       <c r="H58" t="n">
         <v>306235.666666667</v>
@@ -2975,7 +2975,7 @@
         <v>27.08</v>
       </c>
       <c r="G59" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-15637</v>
       </c>
       <c r="H59" t="n">
         <v>307583</v>
@@ -3007,7 +3007,7 @@
         <v>27.16</v>
       </c>
       <c r="G60" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-15443.3333333333</v>
       </c>
       <c r="H60" t="n">
         <v>308733.333333333</v>
@@ -3039,7 +3039,7 @@
         <v>27.24</v>
       </c>
       <c r="G61" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-15249.6666666667</v>
       </c>
       <c r="H61" t="n">
         <v>309883.666666667</v>
@@ -3071,7 +3071,7 @@
         <v>27.5</v>
       </c>
       <c r="G62" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-15056</v>
       </c>
       <c r="H62" t="n">
         <v>311034</v>
@@ -3103,7 +3103,7 @@
         <v>27.56</v>
       </c>
       <c r="G63" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-14226</v>
       </c>
       <c r="H63" t="n">
         <v>312104.333333333</v>
@@ -3135,7 +3135,7 @@
         <v>27.57</v>
       </c>
       <c r="G64" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-13396</v>
       </c>
       <c r="H64" t="n">
         <v>313174.666666667</v>
@@ -3167,7 +3167,7 @@
         <v>27.59</v>
       </c>
       <c r="G65" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-12566</v>
       </c>
       <c r="H65" t="n">
         <v>314245</v>
@@ -3199,7 +3199,7 @@
         <v>27.48</v>
       </c>
       <c r="G66" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-11441.3333333333</v>
       </c>
       <c r="H66" t="n">
         <v>315233.333333333</v>
@@ -3231,7 +3231,7 @@
         <v>27.41</v>
       </c>
       <c r="G67" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-10316.6666666667</v>
       </c>
       <c r="H67" t="n">
         <v>316221.666666667</v>
@@ -3263,7 +3263,7 @@
         <v>27.25</v>
       </c>
       <c r="G68" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-9192</v>
       </c>
       <c r="H68" t="n">
         <v>317210</v>
@@ -3295,7 +3295,7 @@
         <v>27.25</v>
       </c>
       <c r="G69" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-11570.3333333333</v>
       </c>
       <c r="H69" t="n">
         <v>317459</v>
@@ -3327,7 +3327,7 @@
         <v>27.7</v>
       </c>
       <c r="G70" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-13948.6666666667</v>
       </c>
       <c r="H70" t="n">
         <v>317708</v>
@@ -3359,7 +3359,7 @@
         <v>27.8</v>
       </c>
       <c r="G71" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-16327</v>
       </c>
       <c r="H71" t="n">
         <v>317957</v>
@@ -3391,7 +3391,7 @@
         <v>27.84</v>
       </c>
       <c r="G72" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-16710</v>
       </c>
       <c r="H72" t="n">
         <v>318938.666666667</v>
@@ -3423,7 +3423,7 @@
         <v>27.91</v>
       </c>
       <c r="G73" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-17093</v>
       </c>
       <c r="H73" t="n">
         <v>319920.333333333</v>
@@ -3455,7 +3455,7 @@
         <v>28.14</v>
       </c>
       <c r="G74" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-17476</v>
       </c>
       <c r="H74" t="n">
         <v>320902</v>
@@ -3487,7 +3487,7 @@
         <v>28.17</v>
       </c>
       <c r="G75" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-13825</v>
       </c>
       <c r="H75" t="n">
         <v>321917.333333333</v>
@@ -3519,7 +3519,7 @@
         <v>28.14</v>
       </c>
       <c r="G76" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-10174</v>
       </c>
       <c r="H76" t="n">
         <v>322932.666666667</v>
@@ -3551,7 +3551,7 @@
         <v>28.19</v>
       </c>
       <c r="G77" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-6523</v>
       </c>
       <c r="H77" t="n">
         <v>323948</v>
@@ -3583,7 +3583,7 @@
         <v>28.12</v>
       </c>
       <c r="G78" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-8564.66666666667</v>
       </c>
       <c r="H78" t="n">
         <v>324605.333333333</v>
@@ -3615,7 +3615,7 @@
         <v>28.26</v>
       </c>
       <c r="G79" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-10606.3333333333</v>
       </c>
       <c r="H79" t="n">
         <v>325262.666666667</v>
@@ -3647,7 +3647,7 @@
         <v>28.13</v>
       </c>
       <c r="G80" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-12648</v>
       </c>
       <c r="H80" t="n">
         <v>325920</v>
@@ -3679,7 +3679,7 @@
         <v>28.09</v>
       </c>
       <c r="G81" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-11277.3333333333</v>
       </c>
       <c r="H81" t="n">
         <v>327295.333333333</v>
@@ -3711,7 +3711,7 @@
         <v>28.62</v>
       </c>
       <c r="G82" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-9906.66666666667</v>
       </c>
       <c r="H82" t="n">
         <v>328670.666666667</v>
@@ -3743,7 +3743,7 @@
         <v>28.65</v>
       </c>
       <c r="G83" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-8536</v>
       </c>
       <c r="H83" t="n">
         <v>330046</v>
@@ -3775,7 +3775,7 @@
         <v>28.65</v>
       </c>
       <c r="G84" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-11911.3333333333</v>
       </c>
       <c r="H84" t="n">
         <v>327597.666666667</v>
@@ -3807,7 +3807,7 @@
         <v>28.63</v>
       </c>
       <c r="G85" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-15286.6666666667</v>
       </c>
       <c r="H85" t="n">
         <v>325149.333333333</v>
@@ -3839,13 +3839,13 @@
         <v>28.94</v>
       </c>
       <c r="G86" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-18662</v>
       </c>
       <c r="H86" t="n">
         <v>322701</v>
       </c>
       <c r="I86" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-2821</v>
       </c>
       <c r="J86" t="n">
         <v>1.7487</v>
@@ -3871,13 +3871,13 @@
         <v>29.09</v>
       </c>
       <c r="G87" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-15003</v>
       </c>
       <c r="H87" t="n">
         <v>306821.666666667</v>
       </c>
       <c r="I87" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-12412.6666666667</v>
       </c>
       <c r="J87" t="n">
         <v>1.7485</v>
@@ -3903,13 +3903,13 @@
         <v>29.88</v>
       </c>
       <c r="G88" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-11344</v>
       </c>
       <c r="H88" t="n">
         <v>290942.333333333</v>
       </c>
       <c r="I88" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-22004.3333333333</v>
       </c>
       <c r="J88" t="n">
         <v>0.7406</v>
@@ -3935,13 +3935,13 @@
         <v>31.14</v>
       </c>
       <c r="G89" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-7685</v>
       </c>
       <c r="H89" t="n">
         <v>275063</v>
       </c>
       <c r="I89" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-31596</v>
       </c>
       <c r="J89" t="n">
         <v>0.2341</v>
@@ -3967,13 +3967,13 @@
         <v>30.97</v>
       </c>
       <c r="G90" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-9543.66666666667</v>
       </c>
       <c r="H90" t="n">
         <v>287921.333333333</v>
       </c>
       <c r="I90" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-35684.3333333333</v>
       </c>
       <c r="J90" t="n">
         <v>0.2379</v>
@@ -3999,13 +3999,13 @@
         <v>30.29</v>
       </c>
       <c r="G91" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-11402.3333333333</v>
       </c>
       <c r="H91" t="n">
         <v>300779.666666667</v>
       </c>
       <c r="I91" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-39772.6666666667</v>
       </c>
       <c r="J91" t="n">
         <v>0.2327</v>
@@ -4031,13 +4031,13 @@
         <v>29.96</v>
       </c>
       <c r="G92" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-13261</v>
       </c>
       <c r="H92" t="n">
         <v>313638</v>
       </c>
       <c r="I92" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-43861</v>
       </c>
       <c r="J92" t="n">
         <v>0.2407</v>
@@ -4063,13 +4063,13 @@
         <v>29.87</v>
       </c>
       <c r="G93" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-11497</v>
       </c>
       <c r="H93" t="n">
         <v>314590.333333333</v>
       </c>
       <c r="I93" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-34472.3333333333</v>
       </c>
       <c r="J93" t="n">
         <v>0.2337</v>
@@ -4095,13 +4095,13 @@
         <v>30.05</v>
       </c>
       <c r="G94" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-9733</v>
       </c>
       <c r="H94" t="n">
         <v>315542.666666667</v>
       </c>
       <c r="I94" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-25083.6666666667</v>
       </c>
       <c r="J94" t="n">
         <v>0.2181</v>
@@ -4127,13 +4127,13 @@
         <v>30.26</v>
       </c>
       <c r="G95" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-7969</v>
       </c>
       <c r="H95" t="n">
         <v>316495</v>
       </c>
       <c r="I95" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-15695</v>
       </c>
       <c r="J95" t="n">
         <v>0.2337</v>
@@ -4159,13 +4159,13 @@
         <v>30.12</v>
       </c>
       <c r="G96" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-5382.33333333333</v>
       </c>
       <c r="H96" t="n">
         <v>317690</v>
       </c>
       <c r="I96" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-16360</v>
       </c>
       <c r="J96" t="n">
         <v>0.2336</v>
@@ -4191,13 +4191,13 @@
         <v>30.18</v>
       </c>
       <c r="G97" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-2795.66666666667</v>
       </c>
       <c r="H97" t="n">
         <v>318885</v>
       </c>
       <c r="I97" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-17025</v>
       </c>
       <c r="J97" t="n">
         <v>0.1741</v>
@@ -4223,13 +4223,13 @@
         <v>30.75</v>
       </c>
       <c r="G98" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-209</v>
       </c>
       <c r="H98" t="n">
         <v>320080</v>
       </c>
       <c r="I98" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-17690</v>
       </c>
       <c r="J98" t="n">
         <v>0.1826</v>
@@ -4255,13 +4255,13 @@
         <v>30.63</v>
       </c>
       <c r="G99" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-929.666666666667</v>
       </c>
       <c r="H99" t="n">
         <v>320429.666666667</v>
       </c>
       <c r="I99" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-10240.3333333333</v>
       </c>
       <c r="J99" t="n">
         <v>0.2143</v>
@@ -4287,13 +4287,13 @@
         <v>30.46</v>
       </c>
       <c r="G100" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-1650.33333333333</v>
       </c>
       <c r="H100" t="n">
         <v>320779.333333333</v>
       </c>
       <c r="I100" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-2790.66666666667</v>
       </c>
       <c r="J100" t="n">
         <v>0.1529</v>
@@ -4319,7 +4319,7 @@
         <v>30.72</v>
       </c>
       <c r="G101" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-2371</v>
       </c>
       <c r="H101" t="n">
         <v>321129</v>
@@ -4351,13 +4351,13 @@
         <v>30.52</v>
       </c>
       <c r="G102" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-2864.66666666667</v>
       </c>
       <c r="H102" t="n">
         <v>327517.666666667</v>
       </c>
       <c r="I102" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-787.333333333333</v>
       </c>
       <c r="J102" t="n">
         <v>0.1872</v>
@@ -4383,13 +4383,13 @@
         <v>30.29</v>
       </c>
       <c r="G103" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-3358.33333333333</v>
       </c>
       <c r="H103" t="n">
         <v>333906.333333333</v>
       </c>
       <c r="I103" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-6233.66666666667</v>
       </c>
       <c r="J103" t="n">
         <v>0.1873</v>
@@ -4415,13 +4415,13 @@
         <v>30.33</v>
       </c>
       <c r="G104" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-3852</v>
       </c>
       <c r="H104" t="n">
         <v>340295</v>
       </c>
       <c r="I104" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-11680</v>
       </c>
       <c r="J104" t="n">
         <v>0.193</v>
@@ -4447,13 +4447,13 @@
         <v>30.43</v>
       </c>
       <c r="G105" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-2673.66666666667</v>
       </c>
       <c r="H105" t="n">
         <v>342240.333333333</v>
       </c>
       <c r="I105" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-5080</v>
       </c>
       <c r="J105" t="n">
         <v>0.2026</v>
@@ -4479,7 +4479,7 @@
         <v>30.87</v>
       </c>
       <c r="G106" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-1495.33333333333</v>
       </c>
       <c r="H106" t="n">
         <v>344185.666666667</v>
@@ -4511,7 +4511,7 @@
         <v>30.87</v>
       </c>
       <c r="G107" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-317</v>
       </c>
       <c r="H107" t="n">
         <v>346131</v>
@@ -4735,7 +4735,7 @@
         <v>31.64</v>
       </c>
       <c r="G114" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-50.333333333333</v>
       </c>
       <c r="H114" t="n">
         <v>369378.666666667</v>
@@ -4767,7 +4767,7 @@
         <v>31.8</v>
       </c>
       <c r="G115" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-4932.66666666667</v>
       </c>
       <c r="H115" t="n">
         <v>370365.333333333</v>
@@ -4799,7 +4799,7 @@
         <v>31.65</v>
       </c>
       <c r="G116" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-9815</v>
       </c>
       <c r="H116" t="n">
         <v>371352</v>
@@ -4831,7 +4831,7 @@
         <v>31.91</v>
       </c>
       <c r="G117" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-9227.66666666667</v>
       </c>
       <c r="H117" t="n">
         <v>373025</v>
@@ -4863,7 +4863,7 @@
         <v>32.38</v>
       </c>
       <c r="G118" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-8640.33333333333</v>
       </c>
       <c r="H118" t="n">
         <v>374698</v>
@@ -4895,7 +4895,7 @@
         <v>32.52</v>
       </c>
       <c r="G119" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-8053</v>
       </c>
       <c r="H119" t="n">
         <v>376371</v>
@@ -4927,7 +4927,7 @@
         <v>32.71</v>
       </c>
       <c r="G120" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-7424</v>
       </c>
       <c r="H120" t="n">
         <v>378986.333333333</v>
@@ -4959,7 +4959,7 @@
         <v>32.67</v>
       </c>
       <c r="G121" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-6795</v>
       </c>
       <c r="H121" t="n">
         <v>381601.666666667</v>
@@ -4991,7 +4991,7 @@
         <v>33.01</v>
       </c>
       <c r="G122" t="n">
-        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000001</v>
+        <v>-6166</v>
       </c>
       <c r="H122" t="n">
         <v>384217</v>

</xml_diff>